<commit_message>
Week 9 & 10
</commit_message>
<xml_diff>
--- a/files/2021 Charts IN.xlsx
+++ b/files/2021 Charts IN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylmp\Documents\[!] PROJETS PERSONNELS\[MUSIC] 2021 Charts\music_charts\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676ACC8A-9B08-44EF-9043-53FBC1A8ACCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3EFEDA0-9640-4CC6-9286-A4E06B70F40C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{54C79188-7736-4F11-96D1-FC3D6773F7C8}"/>
   </bookViews>
@@ -16,19 +16,28 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$L$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$L$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="702">
   <si>
     <t>Artist</t>
   </si>
@@ -1437,9 +1446,6 @@
     <t>Daft Punk, RetroVision</t>
   </si>
   <si>
-    <t>Harder, Better, Faster, Stronger (RetroVision Remix)</t>
-  </si>
-  <si>
     <t>On My Mind (Chime Mix)</t>
   </si>
   <si>
@@ -1798,6 +1804,345 @@
   </si>
   <si>
     <t>nocopyrightsounds/castion-banger-machine-ncs-release</t>
+  </si>
+  <si>
+    <t>Kaskade, Ella Vos</t>
+  </si>
+  <si>
+    <t>Miles To Go</t>
+  </si>
+  <si>
+    <t>Monstercat Silk, Monstercat</t>
+  </si>
+  <si>
+    <t>Flay!</t>
+  </si>
+  <si>
+    <t>Eunoia</t>
+  </si>
+  <si>
+    <t>Blossoms Asia, Diverge Music Group</t>
+  </si>
+  <si>
+    <t>Dirty Palm, CRVN</t>
+  </si>
+  <si>
+    <t>Alibi</t>
+  </si>
+  <si>
+    <t>LFpJQYtIP-E</t>
+  </si>
+  <si>
+    <t>U6T8PJLkzjI</t>
+  </si>
+  <si>
+    <t>ef-v9MvG2kQ</t>
+  </si>
+  <si>
+    <t>oY9ZcbLHJQQ</t>
+  </si>
+  <si>
+    <t>4fYzzgF4JC0</t>
+  </si>
+  <si>
+    <t>DORkOKSxaBE</t>
+  </si>
+  <si>
+    <t>LSfhaxAZGzw</t>
+  </si>
+  <si>
+    <t>JthLcCcgjy4</t>
+  </si>
+  <si>
+    <t>SAzViYJQ7R4</t>
+  </si>
+  <si>
+    <t>2llcuhz5</t>
+  </si>
+  <si>
+    <t>monstercat/kaskade-ella-vos-miles-to-go</t>
+  </si>
+  <si>
+    <t>blossoms-asia/bls026</t>
+  </si>
+  <si>
+    <t>palmkillit/dirty-palm-alibi-feat-crvn</t>
+  </si>
+  <si>
+    <t>Harder, Better, Faster, Stronger (RetroVision Flip)</t>
+  </si>
+  <si>
+    <t>Eyes Closed</t>
+  </si>
+  <si>
+    <t>Don Diablo, JLV, John K</t>
+  </si>
+  <si>
+    <t>Problems</t>
+  </si>
+  <si>
+    <t>Dirty Palm, joegarratt</t>
+  </si>
+  <si>
+    <t>My Eyes</t>
+  </si>
+  <si>
+    <t>Julian Jordan, Guy Arthur</t>
+  </si>
+  <si>
+    <t>Let Me Be The One</t>
+  </si>
+  <si>
+    <t>Citadelle</t>
+  </si>
+  <si>
+    <t>Out Of My Mind</t>
+  </si>
+  <si>
+    <t>Danimal</t>
+  </si>
+  <si>
+    <t>Wolves</t>
+  </si>
+  <si>
+    <t>You Will Know Our Names</t>
+  </si>
+  <si>
+    <t>OVSKY</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Time Machine, HEXAGON</t>
+  </si>
+  <si>
+    <t>Subshock &amp; Evangelos, MIDNIGHT CVLT</t>
+  </si>
+  <si>
+    <t>Beyond The Skies</t>
+  </si>
+  <si>
+    <t>Feel So Dug (VIP Mix)</t>
+  </si>
+  <si>
+    <t>Future House Music</t>
+  </si>
+  <si>
+    <t>Pixel Terror, ESPER, Isaiah Brown</t>
+  </si>
+  <si>
+    <t>Medusa</t>
+  </si>
+  <si>
+    <t>NUZB, Malarkey</t>
+  </si>
+  <si>
+    <t>Miss Me</t>
+  </si>
+  <si>
+    <t>Mike Williams</t>
+  </si>
+  <si>
+    <t>Get Dirty</t>
+  </si>
+  <si>
+    <t>Scars</t>
+  </si>
+  <si>
+    <t>DISTO, Todd Helder</t>
+  </si>
+  <si>
+    <t>DISTODD</t>
+  </si>
+  <si>
+    <t>Trapstep</t>
+  </si>
+  <si>
+    <t>ue5TBGIenYY</t>
+  </si>
+  <si>
+    <t>RTVld1s0gN4</t>
+  </si>
+  <si>
+    <t>DK-hE0v9iyY</t>
+  </si>
+  <si>
+    <t>B9dU0pdzzB8</t>
+  </si>
+  <si>
+    <t>frNkgEhI6GI</t>
+  </si>
+  <si>
+    <t>mLQkHgxIYSE</t>
+  </si>
+  <si>
+    <t>J0TouyZGvlo</t>
+  </si>
+  <si>
+    <t>31gUmk8ycbg</t>
+  </si>
+  <si>
+    <t>s7fxpF1F2FU</t>
+  </si>
+  <si>
+    <t>JyWF66Uj7v0</t>
+  </si>
+  <si>
+    <t>jjuXbup-5Vw</t>
+  </si>
+  <si>
+    <t>O6cI1Yd594c</t>
+  </si>
+  <si>
+    <t>cn6JChLB1J4</t>
+  </si>
+  <si>
+    <t>DYFLsLIL9k8</t>
+  </si>
+  <si>
+    <t>UN27hjZMxhk</t>
+  </si>
+  <si>
+    <t>1ieZq3nn7sE</t>
+  </si>
+  <si>
+    <t>cLlO1KqXHjo</t>
+  </si>
+  <si>
+    <t>nsusgwlr9VA</t>
+  </si>
+  <si>
+    <t>SPGH8w2ipFs</t>
+  </si>
+  <si>
+    <t>d9qGcB36seI</t>
+  </si>
+  <si>
+    <t>p3Bd7p2OqUM</t>
+  </si>
+  <si>
+    <t>XDijaTchlBw</t>
+  </si>
+  <si>
+    <t>9DKQnKUaI5g</t>
+  </si>
+  <si>
+    <t>8UbtoK3moJk</t>
+  </si>
+  <si>
+    <t>3w7L0UInp4g</t>
+  </si>
+  <si>
+    <t>7QhB3EiNyPw</t>
+  </si>
+  <si>
+    <t>zgoTOo-lCgk</t>
+  </si>
+  <si>
+    <t>DXO0X9kefos</t>
+  </si>
+  <si>
+    <t>KUixd4hoXOM</t>
+  </si>
+  <si>
+    <t>YtuMI5R8sBk</t>
+  </si>
+  <si>
+    <t>BPj9XSeZ1mE</t>
+  </si>
+  <si>
+    <t>ev2H3XQC5vw</t>
+  </si>
+  <si>
+    <t>_HjbEZS6rq8</t>
+  </si>
+  <si>
+    <t>VTPzY9s8h6Y</t>
+  </si>
+  <si>
+    <t>tWB8NLC-44Y</t>
+  </si>
+  <si>
+    <t>Blackcode, Jess Sarubbi</t>
+  </si>
+  <si>
+    <t>Cy35h6DF8hY</t>
+  </si>
+  <si>
+    <t>bdB-hYmJpzo</t>
+  </si>
+  <si>
+    <t>dqwfc7f</t>
+  </si>
+  <si>
+    <t>18p8kmup</t>
+  </si>
+  <si>
+    <t>132rhm2f</t>
+  </si>
+  <si>
+    <t>n5lx1px</t>
+  </si>
+  <si>
+    <t>1tg04qd5</t>
+  </si>
+  <si>
+    <t>tsm5b0f</t>
+  </si>
+  <si>
+    <t>1qmzjpnf</t>
+  </si>
+  <si>
+    <t>1rlbrn05</t>
+  </si>
+  <si>
+    <t>1cguyk35</t>
+  </si>
+  <si>
+    <t>23pk6ptp</t>
+  </si>
+  <si>
+    <t>q17r8kf</t>
+  </si>
+  <si>
+    <t>9xwcb7p</t>
+  </si>
+  <si>
+    <t>citadelleoff/out-of-my-mind</t>
+  </si>
+  <si>
+    <t>julianjordan/julian-jordan-guy-arthur-let-me-be-the-one</t>
+  </si>
+  <si>
+    <t>palmkillit/dirty-palm-my-eyes-feat-joegarratt</t>
+  </si>
+  <si>
+    <t>maxximizerecords/danimal-wolves-radio-edit</t>
+  </si>
+  <si>
+    <t>hexagon/ovsky-missing</t>
+  </si>
+  <si>
+    <t>nocopyrightsounds/subshock-evangelos-x-midnight-cvlt-beyond-the-skies-ncs-release</t>
+  </si>
+  <si>
+    <t>futurehousemusic/mo-falk-feel-so-gud-vip-mix</t>
+  </si>
+  <si>
+    <t>monstercat/pixel-terror-esper-isaiah-brown-medusa</t>
+  </si>
+  <si>
+    <t>nuzb/nuzb-malarkey-miss-me</t>
+  </si>
+  <si>
+    <t>musical-freedom/mike-williams-get-dirty</t>
+  </si>
+  <si>
+    <t>maxximizerecords/blackcode-scars-feat-jesse-sarubbi-radio-edit</t>
+  </si>
+  <si>
+    <t>nocopyrightsounds/disto-todd-helder-distodd-ncs-release</t>
   </si>
 </sst>
 </file>
@@ -2296,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE11BB-30C0-4383-BAC4-B91D2977671A}">
-  <dimension ref="A1:L86"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2656,7 @@
     <col min="5" max="5" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="17.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="64.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="79.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="52.7109375" style="21" customWidth="1"/>
     <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -2438,7 +2783,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>12</v>
@@ -2511,7 +2856,7 @@
         <v>112</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L6" s="19"/>
     </row>
@@ -3152,13 +3497,13 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>557</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>558</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>19</v>
@@ -3167,23 +3512,23 @@
         <v>44216</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G27" s="11" t="str">
         <f>"-L-ffGla2r8"</f>
         <v>-L-ffGla2r8</v>
       </c>
       <c r="H27" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="I27" s="9" t="s">
         <v>580</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="J27" s="15" t="s">
         <v>581</v>
       </c>
-      <c r="J27" s="15" t="s">
+      <c r="K27" s="19" t="s">
         <v>582</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>583</v>
       </c>
       <c r="L27" s="19"/>
     </row>
@@ -3419,37 +3764,37 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>552</v>
       </c>
       <c r="E35" s="4">
         <v>44218</v>
       </c>
       <c r="F35" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>567</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="H35" s="9" t="s">
         <v>568</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="I35" s="9" t="s">
         <v>569</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="J35" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="J35" s="15" t="s">
+      <c r="K35" s="19" t="s">
         <v>571</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>572</v>
       </c>
       <c r="L35" s="19"/>
     </row>
@@ -4147,246 +4492,242 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>302</v>
+        <v>623</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>303</v>
+        <v>624</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>25</v>
+        <v>625</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E57" s="4">
         <v>44232</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>316</v>
+        <v>658</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="H57" s="11"/>
+        <v>659</v>
+      </c>
+      <c r="H57" s="9" t="s">
+        <v>660</v>
+      </c>
       <c r="I57" s="9"/>
       <c r="J57" s="15" t="s">
-        <v>320</v>
+        <v>684</v>
       </c>
       <c r="K57" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="L57" s="19" t="s">
-        <v>327</v>
-      </c>
+        <v>694</v>
+      </c>
+      <c r="L57" s="19"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>440</v>
+        <v>618</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>441</v>
+        <v>619</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>442</v>
+        <v>25</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="E58" s="4">
         <v>44232</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>451</v>
+        <v>640</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>452</v>
-      </c>
-      <c r="H58" s="11"/>
+        <v>641</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>642</v>
+      </c>
       <c r="I58" s="9"/>
       <c r="J58" s="15" t="s">
-        <v>456</v>
+        <v>678</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>460</v>
-      </c>
-      <c r="L58" s="19" t="s">
-        <v>459</v>
-      </c>
+        <v>690</v>
+      </c>
+      <c r="L58" s="19"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>368</v>
+        <v>302</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>370</v>
+        <v>303</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E59" s="4">
-        <v>44237</v>
+        <v>44232</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>378</v>
+        <v>316</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>380</v>
-      </c>
+        <v>317</v>
+      </c>
+      <c r="H59" s="11"/>
       <c r="I59" s="9"/>
       <c r="J59" s="15" t="s">
-        <v>382</v>
+        <v>320</v>
       </c>
       <c r="K59" s="19" t="s">
-        <v>383</v>
-      </c>
-      <c r="L59" s="19"/>
+        <v>326</v>
+      </c>
+      <c r="L59" s="19" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>337</v>
+        <v>440</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>338</v>
+        <v>441</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>47</v>
+        <v>442</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="E60" s="4">
-        <v>44238</v>
+        <v>44232</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>339</v>
+        <v>451</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>340</v>
+        <v>452</v>
       </c>
       <c r="H60" s="11"/>
       <c r="I60" s="9"/>
-      <c r="J60" s="15"/>
+      <c r="J60" s="15" t="s">
+        <v>456</v>
+      </c>
       <c r="K60" s="19" t="s">
-        <v>341</v>
+        <v>460</v>
       </c>
       <c r="L60" s="19" t="s">
-        <v>342</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>417</v>
+        <v>368</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>418</v>
+        <v>370</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>444</v>
+        <v>25</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E61" s="4">
-        <v>44239</v>
+        <v>44237</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>419</v>
+        <v>378</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="H61" s="11"/>
+        <v>379</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>380</v>
+      </c>
       <c r="I61" s="9"/>
       <c r="J61" s="15" t="s">
-        <v>421</v>
-      </c>
-      <c r="K61" s="19"/>
+        <v>382</v>
+      </c>
+      <c r="K61" s="19" t="s">
+        <v>383</v>
+      </c>
       <c r="L61" s="19"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>395</v>
+        <v>337</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>396</v>
+        <v>338</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>397</v>
+        <v>47</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E62" s="4">
-        <v>44239</v>
+        <v>44238</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>398</v>
+        <v>339</v>
       </c>
       <c r="G62" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="H62" s="11" t="s">
-        <v>400</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="H62" s="11"/>
       <c r="I62" s="9"/>
-      <c r="J62" s="15" t="s">
-        <v>401</v>
-      </c>
+      <c r="J62" s="15"/>
       <c r="K62" s="19" t="s">
-        <v>402</v>
+        <v>341</v>
       </c>
       <c r="L62" s="19" t="s">
-        <v>403</v>
+        <v>342</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>395</v>
+        <v>417</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>470</v>
+        <v>418</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>397</v>
+        <v>444</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="E63" s="4">
         <v>44239</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>488</v>
+        <v>419</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="H63" s="9" t="s">
-        <v>449</v>
-      </c>
+        <v>420</v>
+      </c>
+      <c r="H63" s="11"/>
       <c r="I63" s="9"/>
       <c r="J63" s="15" t="s">
-        <v>504</v>
-      </c>
-      <c r="K63" s="19" t="s">
-        <v>510</v>
-      </c>
-      <c r="L63" s="19" t="s">
-        <v>509</v>
-      </c>
+        <v>421</v>
+      </c>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>395</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>445</v>
+        <v>396</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>397</v>
@@ -4398,590 +4739,594 @@
         <v>44239</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>448</v>
+        <v>398</v>
       </c>
       <c r="G64" s="11" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="I64" s="9"/>
       <c r="J64" s="15" t="s">
-        <v>457</v>
+        <v>401</v>
       </c>
       <c r="K64" s="19" t="s">
-        <v>461</v>
+        <v>402</v>
       </c>
       <c r="L64" s="19" t="s">
-        <v>462</v>
+        <v>403</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>141</v>
+        <v>395</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C65" s="2"/>
+        <v>469</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>397</v>
+      </c>
       <c r="D65" s="2" t="s">
-        <v>143</v>
+        <v>19</v>
       </c>
       <c r="E65" s="4">
-        <v>44240</v>
+        <v>44239</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>424</v>
+        <v>487</v>
       </c>
       <c r="G65" s="11" t="s">
-        <v>423</v>
-      </c>
-      <c r="H65" s="11"/>
+        <v>488</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>449</v>
+      </c>
       <c r="I65" s="9"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
+      <c r="J65" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="K65" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="L65" s="19" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>481</v>
+        <v>445</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>45</v>
+        <v>397</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E66" s="4">
-        <v>44246</v>
+        <v>44239</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>500</v>
+        <v>448</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>501</v>
-      </c>
-      <c r="H66" s="9"/>
+        <v>449</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>450</v>
+      </c>
       <c r="I66" s="9"/>
-      <c r="J66" s="15"/>
+      <c r="J66" s="15" t="s">
+        <v>457</v>
+      </c>
       <c r="K66" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="L66" s="19"/>
+        <v>461</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>425</v>
+        <v>141</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>47</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E67" s="4">
-        <v>44246</v>
+        <v>44240</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G67" s="11" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="H67" s="11"/>
       <c r="I67" s="9"/>
       <c r="J67" s="15"/>
-      <c r="K67" s="19" t="s">
-        <v>429</v>
-      </c>
+      <c r="K67" s="19"/>
       <c r="L67" s="19"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>141</v>
+        <v>479</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="C68" s="2"/>
+        <v>480</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D68" s="2" t="s">
-        <v>143</v>
+        <v>29</v>
       </c>
       <c r="E68" s="4">
-        <v>44247</v>
+        <v>44246</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>431</v>
+        <v>499</v>
       </c>
       <c r="G68" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="H68" s="11"/>
+        <v>500</v>
+      </c>
+      <c r="H68" s="9"/>
       <c r="I68" s="9"/>
       <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
+      <c r="K68" s="19" t="s">
+        <v>514</v>
+      </c>
       <c r="L68" s="19"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>468</v>
+        <v>425</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="C69" s="2"/>
+        <v>426</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D69" s="2" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="E69" s="4">
-        <v>44249</v>
+        <v>44246</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>485</v>
+        <v>427</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="H69" s="9" t="s">
-        <v>487</v>
-      </c>
+        <v>428</v>
+      </c>
+      <c r="H69" s="11"/>
       <c r="I69" s="9"/>
-      <c r="J69" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="K69" s="19"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="19" t="s">
+        <v>429</v>
+      </c>
       <c r="L69" s="19"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>405</v>
+        <v>141</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>408</v>
+        <v>143</v>
       </c>
       <c r="E70" s="4">
-        <v>44252</v>
+        <v>44247</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>409</v>
+        <v>431</v>
       </c>
       <c r="G70" s="11" t="s">
-        <v>410</v>
+        <v>432</v>
       </c>
       <c r="H70" s="11"/>
       <c r="I70" s="9"/>
-      <c r="J70" s="15" t="s">
-        <v>413</v>
-      </c>
-      <c r="K70" s="19" t="s">
-        <v>415</v>
-      </c>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
       <c r="L70" s="19"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>404</v>
+        <v>468</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>414</v>
-      </c>
+        <v>610</v>
+      </c>
+      <c r="C71" s="2"/>
       <c r="D71" s="2" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="E71" s="4">
-        <v>44253</v>
+        <v>44249</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>411</v>
+        <v>484</v>
       </c>
       <c r="G71" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="H71" s="11"/>
+        <v>485</v>
+      </c>
+      <c r="H71" s="9" t="s">
+        <v>486</v>
+      </c>
       <c r="I71" s="9"/>
       <c r="J71" s="15" t="s">
-        <v>434</v>
-      </c>
-      <c r="K71" s="19" t="s">
-        <v>416</v>
-      </c>
+        <v>502</v>
+      </c>
+      <c r="K71" s="19"/>
       <c r="L71" s="19"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>523</v>
+        <v>405</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>220</v>
+        <v>407</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>336</v>
+        <v>32</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>42</v>
+        <v>408</v>
       </c>
       <c r="E72" s="4">
-        <v>44253</v>
+        <v>44252</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>542</v>
+        <v>409</v>
       </c>
       <c r="G72" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="H72" s="9" t="s">
-        <v>543</v>
-      </c>
+        <v>410</v>
+      </c>
+      <c r="H72" s="11"/>
       <c r="I72" s="9"/>
       <c r="J72" s="15" t="s">
-        <v>535</v>
+        <v>413</v>
       </c>
       <c r="K72" s="22" t="s">
-        <v>531</v>
-      </c>
-      <c r="L72" s="19" t="s">
-        <v>532</v>
-      </c>
+        <v>415</v>
+      </c>
+      <c r="L72" s="19"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>436</v>
+        <v>406</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>39</v>
+        <v>414</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="E73" s="4">
-        <v>44256</v>
+        <v>44253</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>437</v>
+        <v>411</v>
       </c>
       <c r="G73" s="11" t="s">
-        <v>438</v>
+        <v>412</v>
       </c>
       <c r="H73" s="11"/>
       <c r="I73" s="9"/>
       <c r="J73" s="15" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="L73" s="19"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>446</v>
+        <v>522</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>220</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>336</v>
+      </c>
       <c r="D74" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E74" s="4">
-        <v>44260</v>
+        <v>44253</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>455</v>
+        <v>541</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>454</v>
+        <v>543</v>
       </c>
       <c r="H74" s="9" t="s">
-        <v>453</v>
+        <v>542</v>
       </c>
       <c r="I74" s="9"/>
-      <c r="J74" s="15"/>
+      <c r="J74" s="15" t="s">
+        <v>534</v>
+      </c>
       <c r="K74" s="19" t="s">
-        <v>458</v>
-      </c>
-      <c r="L74" s="19"/>
+        <v>530</v>
+      </c>
+      <c r="L74" s="19" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>478</v>
+        <v>435</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>479</v>
+        <v>436</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E75" s="4">
-        <v>44260</v>
+        <v>44256</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>498</v>
+        <v>437</v>
       </c>
       <c r="G75" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="H75" s="9"/>
+        <v>438</v>
+      </c>
+      <c r="H75" s="11"/>
       <c r="I75" s="9"/>
       <c r="J75" s="15" t="s">
-        <v>506</v>
+        <v>464</v>
       </c>
       <c r="K75" s="19" t="s">
-        <v>514</v>
+        <v>439</v>
       </c>
       <c r="L75" s="19"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>465</v>
+        <v>592</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>466</v>
+        <v>593</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>39</v>
+        <v>594</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>467</v>
+        <v>26</v>
       </c>
       <c r="E76" s="4">
-        <v>44263</v>
+        <v>44260</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>482</v>
+        <v>600</v>
       </c>
       <c r="G76" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="H76" s="9" t="s">
-        <v>484</v>
-      </c>
+        <v>601</v>
+      </c>
+      <c r="H76" s="9"/>
       <c r="I76" s="9"/>
-      <c r="J76" s="15" t="s">
-        <v>502</v>
-      </c>
+      <c r="J76" s="15"/>
       <c r="K76" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="L76" s="19" t="s">
-        <v>508</v>
-      </c>
+        <v>608</v>
+      </c>
+      <c r="L76" s="19"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>520</v>
+        <v>446</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>522</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="C77" s="2"/>
       <c r="D77" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E77" s="4">
-        <v>44266</v>
+        <v>44260</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>538</v>
+        <v>455</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>539</v>
+        <v>454</v>
       </c>
       <c r="H77" s="9" t="s">
-        <v>540</v>
-      </c>
-      <c r="I77" s="9" t="s">
-        <v>541</v>
-      </c>
-      <c r="J77" s="15" t="s">
-        <v>534</v>
-      </c>
+        <v>453</v>
+      </c>
+      <c r="I77" s="9"/>
+      <c r="J77" s="15"/>
       <c r="K77" s="19" t="s">
-        <v>529</v>
-      </c>
-      <c r="L77" s="19" t="s">
-        <v>530</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="L77" s="19"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>476</v>
+        <v>616</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>477</v>
+        <v>617</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="E78" s="4">
-        <v>44266</v>
+        <v>44260</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>495</v>
+        <v>643</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>496</v>
+        <v>644</v>
       </c>
       <c r="H78" s="9" t="s">
-        <v>497</v>
+        <v>645</v>
       </c>
       <c r="I78" s="9"/>
       <c r="J78" s="15" t="s">
-        <v>546</v>
+        <v>679</v>
       </c>
       <c r="K78" s="19" t="s">
-        <v>513</v>
+        <v>691</v>
       </c>
       <c r="L78" s="19"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>518</v>
+        <v>589</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>519</v>
+        <v>590</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>443</v>
+        <v>591</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>140</v>
+        <v>33</v>
       </c>
       <c r="E79" s="4">
-        <v>44267</v>
+        <v>44260</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>524</v>
+        <v>597</v>
       </c>
       <c r="G79" s="11" t="s">
-        <v>525</v>
-      </c>
-      <c r="H79" s="9"/>
+        <v>598</v>
+      </c>
+      <c r="H79" s="9" t="s">
+        <v>599</v>
+      </c>
       <c r="I79" s="9"/>
       <c r="J79" s="15" t="s">
-        <v>526</v>
+        <v>606</v>
       </c>
       <c r="K79" s="19" t="s">
-        <v>527</v>
+        <v>607</v>
       </c>
       <c r="L79" s="19"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>471</v>
+        <v>614</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>335</v>
-      </c>
+        <v>615</v>
+      </c>
+      <c r="C80" s="2"/>
       <c r="D80" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="E80" s="4">
-        <v>44267</v>
+        <v>44260</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>490</v>
+        <v>646</v>
       </c>
       <c r="G80" s="11" t="s">
-        <v>491</v>
+        <v>647</v>
       </c>
       <c r="H80" s="9" t="s">
-        <v>492</v>
-      </c>
-      <c r="I80" s="9"/>
+        <v>648</v>
+      </c>
+      <c r="I80" s="9" t="s">
+        <v>649</v>
+      </c>
       <c r="J80" s="15" t="s">
-        <v>505</v>
+        <v>680</v>
       </c>
       <c r="K80" s="19" t="s">
-        <v>511</v>
+        <v>692</v>
       </c>
       <c r="L80" s="19"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>473</v>
+        <v>612</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C81" s="2"/>
+        <v>613</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D81" s="2" t="s">
-        <v>475</v>
+        <v>50</v>
       </c>
       <c r="E81" s="4">
-        <v>44267</v>
+        <v>44260</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>493</v>
+        <v>650</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>494</v>
-      </c>
-      <c r="H81" s="9"/>
+        <v>651</v>
+      </c>
+      <c r="H81" s="9" t="s">
+        <v>652</v>
+      </c>
       <c r="I81" s="9"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="19" t="s">
-        <v>512</v>
-      </c>
+      <c r="J81" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="K81" s="19"/>
       <c r="L81" s="19"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>560</v>
+        <v>477</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>561</v>
+        <v>478</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>562</v>
+        <v>32</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>563</v>
+        <v>50</v>
       </c>
       <c r="E82" s="4">
-        <v>44267</v>
+        <v>44260</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>586</v>
+        <v>497</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>587</v>
+        <v>498</v>
       </c>
       <c r="H82" s="9"/>
       <c r="I82" s="9"/>
-      <c r="J82" s="15"/>
+      <c r="J82" s="15" t="s">
+        <v>505</v>
+      </c>
       <c r="K82" s="19" t="s">
-        <v>588</v>
+        <v>513</v>
       </c>
       <c r="L82" s="19"/>
     </row>
@@ -4990,20 +5335,20 @@
         <v>141</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>559</v>
+        <v>622</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2" t="s">
         <v>143</v>
       </c>
       <c r="E83" s="4">
-        <v>44268</v>
+        <v>44261</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>584</v>
+        <v>656</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>585</v>
+        <v>657</v>
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
@@ -5013,104 +5358,678 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>516</v>
+        <v>465</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>517</v>
+        <v>466</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>94</v>
+        <v>467</v>
       </c>
       <c r="E84" s="4">
-        <v>44270</v>
+        <v>44263</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>536</v>
+        <v>481</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="H84" s="9"/>
+        <v>482</v>
+      </c>
+      <c r="H84" s="9" t="s">
+        <v>483</v>
+      </c>
       <c r="I84" s="9"/>
       <c r="J84" s="15" t="s">
-        <v>533</v>
+        <v>501</v>
       </c>
       <c r="K84" s="19" t="s">
-        <v>528</v>
-      </c>
-      <c r="L84" s="19"/>
+        <v>506</v>
+      </c>
+      <c r="L84" s="19" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>553</v>
+        <v>519</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>554</v>
+        <v>520</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>555</v>
+        <v>521</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E85" s="4">
-        <v>44274</v>
+        <v>44266</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>574</v>
+        <v>537</v>
       </c>
       <c r="G85" s="11" t="s">
-        <v>575</v>
+        <v>538</v>
       </c>
       <c r="H85" s="9" t="s">
-        <v>576</v>
-      </c>
-      <c r="I85" s="9"/>
+        <v>539</v>
+      </c>
+      <c r="I85" s="9" t="s">
+        <v>540</v>
+      </c>
       <c r="J85" s="15" t="s">
-        <v>577</v>
+        <v>533</v>
       </c>
       <c r="K85" s="19" t="s">
-        <v>578</v>
-      </c>
-      <c r="L85" s="19"/>
+        <v>528</v>
+      </c>
+      <c r="L85" s="19" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>547</v>
+        <v>475</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>549</v>
+        <v>476</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D86" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E86" s="4">
+        <v>44266</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="H86" s="9" t="s">
+        <v>496</v>
+      </c>
+      <c r="I86" s="9"/>
+      <c r="J86" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="K86" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="L86" s="19"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E87" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>524</v>
+      </c>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="K87" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="L87" s="19"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E88" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="H88" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="I88" s="9"/>
+      <c r="J88" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="K88" s="19" t="s">
+        <v>510</v>
+      </c>
+      <c r="L88" s="19"/>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E89" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="19" t="s">
+        <v>511</v>
+      </c>
+      <c r="L89" s="19"/>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="E90" s="4">
+        <v>44267</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="L90" s="19"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E91" s="4">
+        <v>44268</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>584</v>
+      </c>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="19"/>
+      <c r="L91" s="19"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E92" s="4">
+        <v>44270</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>536</v>
+      </c>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="15" t="s">
+        <v>532</v>
+      </c>
+      <c r="K92" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="L92" s="19"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E93" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>666</v>
+      </c>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="K93" s="19" t="s">
+        <v>697</v>
+      </c>
+      <c r="L93" s="19"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" s="4">
+        <v>44273</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>668</v>
+      </c>
+      <c r="H94" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="I94" s="9"/>
+      <c r="J94" s="15" t="s">
+        <v>687</v>
+      </c>
+      <c r="K94" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="L94" s="19"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="4">
+        <v>44274</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>670</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>671</v>
+      </c>
+      <c r="H95" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="I95" s="9"/>
+      <c r="J95" s="15" t="s">
+        <v>688</v>
+      </c>
+      <c r="K95" s="19" t="s">
+        <v>699</v>
+      </c>
+      <c r="L95" s="19"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E96" s="4">
+        <v>44274</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>574</v>
+      </c>
+      <c r="H96" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="I96" s="9"/>
+      <c r="J96" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="K96" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="L96" s="19"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E97" s="4">
+        <v>44274</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>674</v>
+      </c>
+      <c r="H97" s="9"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="15" t="s">
+        <v>689</v>
+      </c>
+      <c r="K97" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="L97" s="19"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" s="4">
+        <v>44277</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>655</v>
+      </c>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="K98" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="L98" s="19"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E99" s="4">
         <v>44277</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="F99" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="G99" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="G86" s="11" t="s">
+      <c r="H99" s="9" t="s">
         <v>565</v>
       </c>
-      <c r="H86" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="I86" s="9"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="19" t="s">
-        <v>573</v>
-      </c>
-      <c r="L86" s="19"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="L99" s="19"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E100" s="4">
+        <v>44279</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="G100" s="11" t="s">
+        <v>664</v>
+      </c>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="15" t="s">
+        <v>685</v>
+      </c>
+      <c r="K100" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="L100" s="19"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E101" s="4">
+        <v>44288</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="G101" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="H101" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="I101" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="J101" s="15"/>
+      <c r="K101" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="L101" s="19"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" s="4">
+        <v>44288</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="G102" s="11"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="15" t="s">
+        <v>682</v>
+      </c>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E103" s="4">
+        <v>44292</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="G103" s="11" t="s">
+        <v>662</v>
+      </c>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="15"/>
+      <c r="K103" s="19" t="s">
+        <v>695</v>
+      </c>
+      <c r="L103" s="19"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="E104" s="4">
+        <v>44295</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G104" s="11" t="s">
+        <v>677</v>
+      </c>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="19" t="s">
+        <v>701</v>
+      </c>
+      <c r="L104" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L86" xr:uid="{8FDDA10C-A993-4E1E-BA2B-64BD684A4CD0}">
+  <autoFilter ref="A1:L104" xr:uid="{8FDDA10C-A993-4E1E-BA2B-64BD684A4CD0}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L68">
       <sortCondition ref="E2:E68"/>
       <sortCondition ref="A2:A68"/>
@@ -5119,10 +6038,10 @@
       <sortCondition ref="D2:D68"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L86">
-    <sortCondition ref="E2:E86"/>
-    <sortCondition ref="B2:B86"/>
-    <sortCondition ref="A2:A86"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L104">
+    <sortCondition ref="E2:E104"/>
+    <sortCondition ref="B2:B104"/>
+    <sortCondition ref="A2:A104"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Week 19 + minor changes
</commit_message>
<xml_diff>
--- a/files/2021 Charts IN.xlsx
+++ b/files/2021 Charts IN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylmp\Documents\[!] PROJETS PERSONNELS\[MUSIC] 2021 Charts\music_charts\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884BB748-5A96-4D91-8940-20CD4155A874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4E3C69-EC62-4367-8EC0-DE529074603C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{54C79188-7736-4F11-96D1-FC3D6773F7C8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$L$157</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$L$163</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="1094">
   <si>
     <t>Artist</t>
   </si>
@@ -2766,9 +2766,6 @@
     <t>hexagon/faith-giving-everything</t>
   </si>
   <si>
-    <t>faithofficial/faith-giving-everything-extended-mix-hexagon</t>
-  </si>
-  <si>
     <t>Bear Grillz, Nevve</t>
   </si>
   <si>
@@ -3087,9 +3084,6 @@
     <t>dyro/memory-bank</t>
   </si>
   <si>
-    <t>/itsbasstian/make-you-mine-1</t>
-  </si>
-  <si>
     <t>itsbasstian/make-you-mine-extended-mix</t>
   </si>
   <si>
@@ -3190,6 +3184,141 @@
   </si>
   <si>
     <t>haywyre/haywyre-wisdom</t>
+  </si>
+  <si>
+    <t>Diversity, Diverge Music Group</t>
+  </si>
+  <si>
+    <t>PhoenixZ, EXABiOS</t>
+  </si>
+  <si>
+    <t>Don't Worry</t>
+  </si>
+  <si>
+    <t>Pixel Terror, Chime, Teminite</t>
+  </si>
+  <si>
+    <t>Sleepless</t>
+  </si>
+  <si>
+    <t>Dirtyphonics</t>
+  </si>
+  <si>
+    <t>Gasoline</t>
+  </si>
+  <si>
+    <t>David Guetta, MORTEN, John Martin</t>
+  </si>
+  <si>
+    <t>Impossible</t>
+  </si>
+  <si>
+    <t>Hardwell, Mitch Crown, Dr Phunk</t>
+  </si>
+  <si>
+    <t>Spaceman (Dr Phunk Remix)</t>
+  </si>
+  <si>
+    <t>Valy Mo, Highup</t>
+  </si>
+  <si>
+    <t>The Rise</t>
+  </si>
+  <si>
+    <t>ceC9C1xLvrU</t>
+  </si>
+  <si>
+    <t>99Ree3gf5mE</t>
+  </si>
+  <si>
+    <t>KcUXPGIJk6Y</t>
+  </si>
+  <si>
+    <t>4AGSRqAdl94</t>
+  </si>
+  <si>
+    <t>fIkmJ0-0m5Q</t>
+  </si>
+  <si>
+    <t>r7h-XG5tF70</t>
+  </si>
+  <si>
+    <t>SHramqeWRaE</t>
+  </si>
+  <si>
+    <t>GcWV6JCU96A</t>
+  </si>
+  <si>
+    <t>70MXvzD2d50</t>
+  </si>
+  <si>
+    <t>ysWcsd0SG88</t>
+  </si>
+  <si>
+    <t>YDzeSueT3Hk</t>
+  </si>
+  <si>
+    <t>pJcrGaWnrGc</t>
+  </si>
+  <si>
+    <t>zhqqcNafowU</t>
+  </si>
+  <si>
+    <t>7mLyio3hn1o</t>
+  </si>
+  <si>
+    <t>Q5yR2hJRK4I</t>
+  </si>
+  <si>
+    <t>t1jjbypUu8w</t>
+  </si>
+  <si>
+    <t>UqrDmmMIQc0</t>
+  </si>
+  <si>
+    <t>nWXL7zSCZkc</t>
+  </si>
+  <si>
+    <t>w91rXCeXWfY</t>
+  </si>
+  <si>
+    <t>jsz4wCEMbls</t>
+  </si>
+  <si>
+    <t>1rm314vp</t>
+  </si>
+  <si>
+    <t>1092dc3p</t>
+  </si>
+  <si>
+    <t>1t3kr08x</t>
+  </si>
+  <si>
+    <t>q1hqjjf</t>
+  </si>
+  <si>
+    <t>divr/div103</t>
+  </si>
+  <si>
+    <t>monstercat/pixel-terror-chime-teminite-sleepless</t>
+  </si>
+  <si>
+    <t>teminite/sleepless</t>
+  </si>
+  <si>
+    <t>disciple/gasoline</t>
+  </si>
+  <si>
+    <t>musical-freedom/david-guetta-morten-ft-john-martin-impossible-radio-edit</t>
+  </si>
+  <si>
+    <t>hardwell/spaceman-dr-phunk-remix-feat</t>
+  </si>
+  <si>
+    <t>musical-freedom/valy-mo-highup-the-rise</t>
+  </si>
+  <si>
+    <t>itsbasstian/make-you-mine-1</t>
   </si>
 </sst>
 </file>
@@ -3689,10 +3818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCE11BB-30C0-4383-BAC4-B91D2977671A}">
-  <dimension ref="A1:L157"/>
+  <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="D127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L151" sqref="L151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7261,13 +7390,13 @@
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>1032</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>1033</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>1034</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>94</v>
@@ -7276,16 +7405,16 @@
         <v>44279</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="H110" s="9"/>
       <c r="I110" s="9"/>
       <c r="J110" s="15"/>
       <c r="K110" s="19" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="L110" s="19"/>
     </row>
@@ -7323,1007 +7452,1009 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>594</v>
+        <v>1050</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="C112" s="2"/>
+        <v>1051</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>1049</v>
+      </c>
       <c r="D112" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E112" s="4">
-        <v>44288</v>
+        <v>44281</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>601</v>
+        <v>1062</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>602</v>
+        <v>1063</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="I112" s="9" t="s">
-        <v>604</v>
-      </c>
-      <c r="J112" s="15" t="s">
-        <v>894</v>
-      </c>
+        <v>1064</v>
+      </c>
+      <c r="I112" s="9"/>
+      <c r="J112" s="15"/>
       <c r="K112" s="19" t="s">
-        <v>608</v>
+        <v>1086</v>
       </c>
       <c r="L112" s="19"/>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>345</v>
+        <v>594</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>595</v>
+      </c>
+      <c r="C113" s="2"/>
       <c r="D113" s="2" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="E113" s="4">
         <v>44288</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="G113" s="11"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="9"/>
+        <v>601</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="H113" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="I113" s="9" t="s">
+        <v>604</v>
+      </c>
       <c r="J113" s="15" t="s">
-        <v>679</v>
-      </c>
-      <c r="K113" s="19"/>
+        <v>894</v>
+      </c>
+      <c r="K113" s="19" t="s">
+        <v>608</v>
+      </c>
       <c r="L113" s="19"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>701</v>
+        <v>345</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>702</v>
+        <v>610</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>703</v>
+        <v>32</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E114" s="4">
         <v>44288</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>725</v>
-      </c>
-      <c r="G114" s="11" t="s">
-        <v>724</v>
-      </c>
+        <v>651</v>
+      </c>
+      <c r="G114" s="11"/>
       <c r="H114" s="9"/>
       <c r="I114" s="9"/>
       <c r="J114" s="15" t="s">
-        <v>743</v>
-      </c>
-      <c r="K114" s="19" t="s">
-        <v>750</v>
-      </c>
+        <v>679</v>
+      </c>
+      <c r="K114" s="19"/>
       <c r="L114" s="19"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>1035</v>
+        <v>701</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>1036</v>
+        <v>702</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1037</v>
+        <v>703</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E115" s="4">
         <v>44288</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>1043</v>
+        <v>725</v>
       </c>
       <c r="G115" s="11" t="s">
-        <v>1044</v>
-      </c>
-      <c r="H115" s="9" t="s">
-        <v>1045</v>
-      </c>
+        <v>724</v>
+      </c>
+      <c r="H115" s="9"/>
       <c r="I115" s="9"/>
       <c r="J115" s="15" t="s">
-        <v>1047</v>
+        <v>743</v>
       </c>
       <c r="K115" s="19" t="s">
-        <v>1050</v>
+        <v>750</v>
       </c>
       <c r="L115" s="19"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>719</v>
+        <v>1033</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="C116" s="22"/>
-      <c r="D116" s="22" t="s">
-        <v>29</v>
+        <v>1034</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E116" s="4">
-        <v>44290</v>
+        <v>44288</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>741</v>
-      </c>
-      <c r="G116" s="11"/>
-      <c r="H116" s="9"/>
+        <v>1041</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>1042</v>
+      </c>
+      <c r="H116" s="9" t="s">
+        <v>1043</v>
+      </c>
       <c r="I116" s="9"/>
-      <c r="J116" s="15"/>
+      <c r="J116" s="15" t="s">
+        <v>1045</v>
+      </c>
       <c r="K116" s="19" t="s">
-        <v>756</v>
+        <v>1048</v>
       </c>
       <c r="L116" s="19"/>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>709</v>
+        <v>719</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="C117" s="22" t="s">
-        <v>39</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="C117" s="22"/>
       <c r="D117" s="22" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E117" s="4">
-        <v>44291</v>
+        <v>44290</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>731</v>
-      </c>
-      <c r="G117" s="11" t="s">
-        <v>732</v>
-      </c>
+        <v>741</v>
+      </c>
+      <c r="G117" s="11"/>
       <c r="H117" s="9"/>
       <c r="I117" s="9"/>
-      <c r="J117" s="15" t="s">
-        <v>745</v>
-      </c>
+      <c r="J117" s="15"/>
       <c r="K117" s="19" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
       <c r="L117" s="19"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>625</v>
+        <v>709</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>109</v>
+        <v>710</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D118" s="22" t="s">
+        <v>50</v>
       </c>
       <c r="E118" s="4">
-        <v>44292</v>
+        <v>44291</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>659</v>
+        <v>731</v>
       </c>
       <c r="G118" s="11" t="s">
-        <v>660</v>
+        <v>732</v>
       </c>
       <c r="H118" s="9"/>
       <c r="I118" s="9"/>
       <c r="J118" s="15" t="s">
-        <v>995</v>
+        <v>745</v>
       </c>
       <c r="K118" s="19" t="s">
-        <v>692</v>
+        <v>753</v>
       </c>
       <c r="L118" s="19"/>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>637</v>
+        <v>109</v>
       </c>
       <c r="E119" s="4">
-        <v>44295</v>
+        <v>44292</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="H119" s="9"/>
       <c r="I119" s="9"/>
-      <c r="J119" s="15"/>
+      <c r="J119" s="15" t="s">
+        <v>994</v>
+      </c>
       <c r="K119" s="19" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="L119" s="19"/>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>961</v>
+        <v>635</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>962</v>
+        <v>636</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>960</v>
+        <v>47</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>26</v>
+        <v>637</v>
       </c>
       <c r="E120" s="4">
         <v>44295</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>976</v>
+        <v>673</v>
       </c>
       <c r="G120" s="11" t="s">
-        <v>977</v>
-      </c>
-      <c r="H120" s="9" t="s">
-        <v>978</v>
-      </c>
-      <c r="I120" s="9" t="s">
-        <v>979</v>
-      </c>
-      <c r="J120" s="15" t="s">
-        <v>983</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="15"/>
       <c r="K120" s="19" t="s">
-        <v>984</v>
+        <v>698</v>
       </c>
       <c r="L120" s="19"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>711</v>
+        <v>960</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="C121" s="22" t="s">
-        <v>713</v>
-      </c>
-      <c r="D121" s="22" t="s">
-        <v>714</v>
+        <v>961</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E121" s="4">
         <v>44295</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>733</v>
+        <v>975</v>
       </c>
       <c r="G121" s="11" t="s">
-        <v>734</v>
+        <v>976</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>1038</v>
-      </c>
-      <c r="I121" s="9"/>
+        <v>977</v>
+      </c>
+      <c r="I121" s="9" t="s">
+        <v>978</v>
+      </c>
       <c r="J121" s="15" t="s">
-        <v>746</v>
+        <v>982</v>
       </c>
       <c r="K121" s="19" t="s">
-        <v>754</v>
+        <v>983</v>
       </c>
       <c r="L121" s="19"/>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>141</v>
+        <v>711</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="C122" s="22"/>
+        <v>712</v>
+      </c>
+      <c r="C122" s="22" t="s">
+        <v>713</v>
+      </c>
       <c r="D122" s="22" t="s">
-        <v>143</v>
+        <v>714</v>
       </c>
       <c r="E122" s="4">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="G122" s="11" t="s">
-        <v>740</v>
-      </c>
-      <c r="H122" s="9"/>
+        <v>734</v>
+      </c>
+      <c r="H122" s="9" t="s">
+        <v>1036</v>
+      </c>
       <c r="I122" s="9"/>
-      <c r="J122" s="15"/>
-      <c r="K122" s="19"/>
+      <c r="J122" s="15" t="s">
+        <v>746</v>
+      </c>
+      <c r="K122" s="19" t="s">
+        <v>754</v>
+      </c>
       <c r="L122" s="19"/>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>850</v>
+        <v>1060</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>851</v>
-      </c>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2" t="s">
-        <v>852</v>
+        <v>1061</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D123" s="22" t="s">
+        <v>232</v>
       </c>
       <c r="E123" s="4">
-        <v>44300</v>
+        <v>44295</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>881</v>
+        <v>1079</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>882</v>
-      </c>
-      <c r="H123" s="9"/>
+        <v>1080</v>
+      </c>
+      <c r="H123" s="9" t="s">
+        <v>1081</v>
+      </c>
       <c r="I123" s="9"/>
-      <c r="J123" s="15"/>
+      <c r="J123" s="15" t="s">
+        <v>1085</v>
+      </c>
       <c r="K123" s="19" t="s">
-        <v>883</v>
+        <v>1092</v>
       </c>
       <c r="L123" s="19"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>699</v>
+        <v>141</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>700</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>29</v>
+        <v>718</v>
+      </c>
+      <c r="C124" s="22"/>
+      <c r="D124" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="E124" s="4">
-        <v>44301</v>
+        <v>44296</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>721</v>
+        <v>739</v>
       </c>
       <c r="G124" s="11" t="s">
-        <v>722</v>
-      </c>
-      <c r="H124" s="9" t="s">
-        <v>723</v>
-      </c>
+        <v>740</v>
+      </c>
+      <c r="H124" s="9"/>
       <c r="I124" s="9"/>
-      <c r="J124" s="15" t="s">
-        <v>742</v>
-      </c>
-      <c r="K124" s="19" t="s">
-        <v>748</v>
-      </c>
+      <c r="J124" s="15"/>
+      <c r="K124" s="19"/>
       <c r="L124" s="19"/>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>435</v>
+        <v>850</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>849</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>851</v>
+      </c>
+      <c r="C125" s="2"/>
       <c r="D125" s="2" t="s">
-        <v>53</v>
+        <v>852</v>
       </c>
       <c r="E125" s="4">
-        <v>44301</v>
+        <v>44300</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
       <c r="G125" s="11" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="H125" s="9"/>
       <c r="I125" s="9"/>
       <c r="J125" s="15"/>
       <c r="K125" s="19" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="L125" s="19"/>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>915</v>
+        <v>699</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>916</v>
+        <v>700</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>335</v>
+        <v>25</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E126" s="4">
-        <v>44302</v>
+        <v>44301</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>922</v>
+        <v>721</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>923</v>
+        <v>722</v>
       </c>
       <c r="H126" s="9" t="s">
-        <v>924</v>
-      </c>
-      <c r="I126" s="9" t="s">
-        <v>925</v>
-      </c>
+        <v>723</v>
+      </c>
+      <c r="I126" s="9"/>
       <c r="J126" s="15" t="s">
-        <v>927</v>
+        <v>742</v>
       </c>
       <c r="K126" s="19" t="s">
-        <v>930</v>
+        <v>748</v>
       </c>
       <c r="L126" s="19"/>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>759</v>
+        <v>435</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>760</v>
+        <v>849</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E127" s="4">
-        <v>44306</v>
+        <v>44301</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>773</v>
+        <v>878</v>
       </c>
       <c r="G127" s="11" t="s">
-        <v>774</v>
-      </c>
-      <c r="H127" s="9" t="s">
-        <v>775</v>
-      </c>
+        <v>879</v>
+      </c>
+      <c r="H127" s="9"/>
       <c r="I127" s="9"/>
-      <c r="J127" s="15" t="s">
-        <v>785</v>
-      </c>
+      <c r="J127" s="15"/>
       <c r="K127" s="19" t="s">
-        <v>790</v>
+        <v>880</v>
       </c>
       <c r="L127" s="19"/>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>895</v>
+        <v>914</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>848</v>
+        <v>915</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>47</v>
+        <v>335</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E128" s="4">
-        <v>44306</v>
+        <v>44302</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>873</v>
+        <v>921</v>
       </c>
       <c r="G128" s="11" t="s">
-        <v>874</v>
+        <v>922</v>
       </c>
       <c r="H128" s="9" t="s">
-        <v>875</v>
-      </c>
-      <c r="I128" s="9"/>
+        <v>923</v>
+      </c>
+      <c r="I128" s="9" t="s">
+        <v>924</v>
+      </c>
       <c r="J128" s="15" t="s">
-        <v>876</v>
+        <v>926</v>
       </c>
       <c r="K128" s="19" t="s">
-        <v>877</v>
+        <v>929</v>
       </c>
       <c r="L128" s="19"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>804</v>
+        <v>759</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>805</v>
-      </c>
-      <c r="C129" s="2"/>
+        <v>760</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="D129" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="E129" s="4">
         <v>44306</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>832</v>
-      </c>
-      <c r="G129" s="11"/>
-      <c r="H129" s="9"/>
+        <v>773</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>774</v>
+      </c>
+      <c r="H129" s="9" t="s">
+        <v>775</v>
+      </c>
       <c r="I129" s="9"/>
       <c r="J129" s="15" t="s">
-        <v>833</v>
-      </c>
-      <c r="K129" s="19"/>
+        <v>785</v>
+      </c>
+      <c r="K129" s="19" t="s">
+        <v>790</v>
+      </c>
       <c r="L129" s="19"/>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>846</v>
+        <v>895</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E130" s="4">
-        <v>44307</v>
+        <v>44306</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>870</v>
-      </c>
-      <c r="H130" s="9"/>
+        <v>874</v>
+      </c>
+      <c r="H130" s="9" t="s">
+        <v>875</v>
+      </c>
       <c r="I130" s="9"/>
       <c r="J130" s="15" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="K130" s="19" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="L130" s="19"/>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>761</v>
+        <v>804</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>762</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>335</v>
-      </c>
+        <v>805</v>
+      </c>
+      <c r="C131" s="2"/>
       <c r="D131" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E131" s="4">
-        <v>44308</v>
+        <v>44306</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>776</v>
-      </c>
-      <c r="G131" s="11" t="s">
-        <v>777</v>
-      </c>
-      <c r="H131" s="9" t="str">
-        <f>"-vnPfhtfzmk"</f>
-        <v>-vnPfhtfzmk</v>
-      </c>
-      <c r="I131" s="9" t="s">
-        <v>778</v>
-      </c>
+        <v>832</v>
+      </c>
+      <c r="G131" s="11"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
       <c r="J131" s="15" t="s">
-        <v>786</v>
-      </c>
-      <c r="K131" s="19" t="s">
-        <v>791</v>
-      </c>
+        <v>833</v>
+      </c>
+      <c r="K131" s="19"/>
       <c r="L131" s="19"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>233</v>
+        <v>846</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>798</v>
+        <v>847</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>234</v>
+        <v>117</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>799</v>
+        <v>29</v>
       </c>
       <c r="E132" s="4">
-        <v>44309</v>
+        <v>44307</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>819</v>
+        <v>869</v>
       </c>
       <c r="G132" s="11" t="s">
-        <v>820</v>
+        <v>870</v>
       </c>
       <c r="H132" s="9"/>
       <c r="I132" s="9"/>
       <c r="J132" s="15" t="s">
-        <v>824</v>
+        <v>871</v>
       </c>
       <c r="K132" s="19" t="s">
-        <v>825</v>
+        <v>872</v>
       </c>
       <c r="L132" s="19"/>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>801</v>
+        <v>761</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>802</v>
+        <v>762</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>803</v>
+        <v>335</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E133" s="4">
-        <v>44309</v>
+        <v>44308</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>828</v>
+        <v>776</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>829</v>
-      </c>
-      <c r="H133" s="9" t="s">
-        <v>830</v>
-      </c>
-      <c r="I133" s="9"/>
-      <c r="J133" s="15"/>
+        <v>777</v>
+      </c>
+      <c r="H133" s="9" t="str">
+        <f>"-vnPfhtfzmk"</f>
+        <v>-vnPfhtfzmk</v>
+      </c>
+      <c r="I133" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="J133" s="15" t="s">
+        <v>786</v>
+      </c>
       <c r="K133" s="19" t="s">
-        <v>831</v>
+        <v>791</v>
       </c>
       <c r="L133" s="19"/>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>477</v>
+        <v>233</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>25</v>
+        <v>234</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>50</v>
+        <v>799</v>
       </c>
       <c r="E134" s="4">
         <v>44309</v>
       </c>
       <c r="F134" s="9" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G134" s="11" t="s">
-        <v>822</v>
-      </c>
-      <c r="H134" s="9" t="s">
-        <v>823</v>
-      </c>
+        <v>820</v>
+      </c>
+      <c r="H134" s="9"/>
       <c r="I134" s="9"/>
       <c r="J134" s="15" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="K134" s="19" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="L134" s="19"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>796</v>
+        <v>801</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>797</v>
+        <v>802</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>25</v>
+        <v>803</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E135" s="4">
-        <v>44315</v>
+        <v>44309</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>814</v>
+        <v>828</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>815</v>
+        <v>829</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>816</v>
+        <v>830</v>
       </c>
       <c r="I135" s="9"/>
-      <c r="J135" s="15" t="s">
-        <v>817</v>
-      </c>
+      <c r="J135" s="15"/>
       <c r="K135" s="19" t="s">
-        <v>818</v>
+        <v>831</v>
       </c>
       <c r="L135" s="19"/>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>896</v>
+        <v>477</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>897</v>
-      </c>
-      <c r="C136" s="2"/>
+        <v>800</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D136" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="E136" s="4">
-        <v>44316</v>
+        <v>44309</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>899</v>
+        <v>821</v>
       </c>
       <c r="G136" s="11" t="s">
-        <v>900</v>
-      </c>
-      <c r="H136" s="11" t="s">
-        <v>898</v>
-      </c>
-      <c r="I136" s="9" t="s">
-        <v>901</v>
-      </c>
+        <v>822</v>
+      </c>
+      <c r="H136" s="9" t="s">
+        <v>823</v>
+      </c>
+      <c r="I136" s="9"/>
       <c r="J136" s="15" t="s">
-        <v>1018</v>
+        <v>826</v>
       </c>
       <c r="K136" s="19" t="s">
-        <v>902</v>
+        <v>827</v>
       </c>
       <c r="L136" s="19"/>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>951</v>
+        <v>796</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>952</v>
+        <v>797</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E137" s="4">
-        <v>44316</v>
+        <v>44315</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>964</v>
+        <v>814</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>963</v>
+        <v>815</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>965</v>
-      </c>
-      <c r="I137" s="9" t="s">
-        <v>966</v>
-      </c>
+        <v>816</v>
+      </c>
+      <c r="I137" s="9"/>
       <c r="J137" s="15" t="s">
-        <v>980</v>
+        <v>817</v>
       </c>
       <c r="K137" s="19" t="s">
-        <v>985</v>
+        <v>818</v>
       </c>
       <c r="L137" s="19"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>347</v>
+        <v>896</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>795</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="C138" s="2"/>
       <c r="D138" s="2" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="E138" s="4">
         <v>44316</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>810</v>
+        <v>899</v>
       </c>
       <c r="G138" s="11" t="s">
-        <v>811</v>
-      </c>
-      <c r="H138" s="9"/>
-      <c r="I138" s="9"/>
+        <v>900</v>
+      </c>
+      <c r="H138" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>901</v>
+      </c>
       <c r="J138" s="15" t="s">
-        <v>812</v>
+        <v>1016</v>
       </c>
       <c r="K138" s="19" t="s">
-        <v>813</v>
+        <v>902</v>
       </c>
       <c r="L138" s="19"/>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>845</v>
+        <v>950</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>932</v>
-      </c>
-      <c r="C139" s="2"/>
+        <v>951</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D139" s="2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="E139" s="4">
-        <v>44320</v>
+        <v>44316</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>865</v>
+        <v>963</v>
       </c>
       <c r="G139" s="11" t="s">
-        <v>866</v>
+        <v>962</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>867</v>
-      </c>
-      <c r="I139" s="9"/>
-      <c r="J139" s="15"/>
+        <v>964</v>
+      </c>
+      <c r="I139" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="J139" s="15" t="s">
+        <v>979</v>
+      </c>
       <c r="K139" s="19" t="s">
-        <v>868</v>
+        <v>984</v>
       </c>
       <c r="L139" s="19"/>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>843</v>
+        <v>347</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>844</v>
+        <v>795</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="E140" s="4">
-        <v>44322</v>
+        <v>44316</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>860</v>
+        <v>810</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>861</v>
+        <v>811</v>
       </c>
       <c r="H140" s="9"/>
       <c r="I140" s="9"/>
       <c r="J140" s="15" t="s">
-        <v>862</v>
+        <v>812</v>
       </c>
       <c r="K140" s="19" t="s">
-        <v>863</v>
-      </c>
-      <c r="L140" s="19" t="s">
-        <v>864</v>
-      </c>
+        <v>813</v>
+      </c>
+      <c r="L140" s="19"/>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>48</v>
+        <v>845</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>937</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>931</v>
+      </c>
+      <c r="C141" s="2"/>
       <c r="D141" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="E141" s="4">
-        <v>44322</v>
+        <v>44320</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>942</v>
+        <v>865</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>943</v>
-      </c>
-      <c r="H141" s="9"/>
+        <v>866</v>
+      </c>
+      <c r="H141" s="9" t="s">
+        <v>867</v>
+      </c>
       <c r="I141" s="9"/>
-      <c r="J141" s="15" t="s">
-        <v>946</v>
-      </c>
+      <c r="J141" s="15"/>
       <c r="K141" s="19" t="s">
-        <v>950</v>
+        <v>868</v>
       </c>
       <c r="L141" s="19"/>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>841</v>
+        <v>844</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>842</v>
+        <v>39</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E142" s="4">
-        <v>44323</v>
+        <v>44322</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="G142" s="11" t="s">
-        <v>857</v>
+        <v>861</v>
       </c>
       <c r="H142" s="9"/>
       <c r="I142" s="9"/>
       <c r="J142" s="15" t="s">
-        <v>858</v>
+        <v>862</v>
       </c>
       <c r="K142" s="19" t="s">
-        <v>859</v>
-      </c>
-      <c r="L142" s="19"/>
+        <v>863</v>
+      </c>
+      <c r="L142" s="19" t="s">
+        <v>864</v>
+      </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>999</v>
+        <v>48</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>1000</v>
+        <v>936</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>32</v>
@@ -8332,60 +8463,62 @@
         <v>29</v>
       </c>
       <c r="E143" s="4">
-        <v>44323</v>
+        <v>44322</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>1007</v>
+        <v>941</v>
       </c>
       <c r="G143" s="11" t="s">
-        <v>1008</v>
+        <v>942</v>
       </c>
       <c r="H143" s="9"/>
       <c r="I143" s="9"/>
       <c r="J143" s="15" t="s">
-        <v>1013</v>
-      </c>
-      <c r="K143" s="19"/>
+        <v>945</v>
+      </c>
+      <c r="K143" s="19" t="s">
+        <v>949</v>
+      </c>
       <c r="L143" s="19"/>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>935</v>
+        <v>840</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>936</v>
+        <v>841</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>39</v>
+        <v>842</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="E144" s="4">
-        <v>44327</v>
+        <v>44323</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>940</v>
+        <v>856</v>
       </c>
       <c r="G144" s="11" t="s">
-        <v>941</v>
+        <v>857</v>
       </c>
       <c r="H144" s="9"/>
       <c r="I144" s="9"/>
       <c r="J144" s="15" t="s">
-        <v>945</v>
+        <v>858</v>
       </c>
       <c r="K144" s="19" t="s">
-        <v>949</v>
+        <v>859</v>
       </c>
       <c r="L144" s="19"/>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>903</v>
+        <v>998</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>904</v>
+        <v>999</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>32</v>
@@ -8394,352 +8527,346 @@
         <v>29</v>
       </c>
       <c r="E145" s="4">
-        <v>44329</v>
+        <v>44323</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>905</v>
+        <v>1006</v>
       </c>
       <c r="G145" s="11" t="s">
-        <v>906</v>
+        <v>1007</v>
       </c>
       <c r="H145" s="9"/>
       <c r="I145" s="9"/>
       <c r="J145" s="15" t="s">
-        <v>907</v>
-      </c>
-      <c r="K145" s="19" t="s">
-        <v>909</v>
-      </c>
-      <c r="L145" s="19" t="s">
-        <v>908</v>
-      </c>
+        <v>1012</v>
+      </c>
+      <c r="K145" s="19"/>
+      <c r="L145" s="19"/>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>913</v>
+        <v>934</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>914</v>
+        <v>935</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>931</v>
+        <v>39</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="E146" s="4">
-        <v>44330</v>
+        <v>44327</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>919</v>
+        <v>939</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>920</v>
-      </c>
-      <c r="H146" s="9" t="s">
-        <v>921</v>
-      </c>
+        <v>940</v>
+      </c>
+      <c r="H146" s="9"/>
       <c r="I146" s="9"/>
       <c r="J146" s="15" t="s">
-        <v>926</v>
+        <v>944</v>
       </c>
       <c r="K146" s="19" t="s">
-        <v>929</v>
+        <v>948</v>
       </c>
       <c r="L146" s="19"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>910</v>
+        <v>903</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>911</v>
+        <v>904</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>912</v>
+        <v>32</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E147" s="4">
-        <v>44330</v>
+        <v>44329</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>917</v>
+        <v>905</v>
       </c>
       <c r="G147" s="11" t="s">
-        <v>918</v>
+        <v>906</v>
       </c>
       <c r="H147" s="9"/>
       <c r="I147" s="9"/>
       <c r="J147" s="15" t="s">
-        <v>944</v>
+        <v>907</v>
       </c>
       <c r="K147" s="19" t="s">
-        <v>928</v>
+        <v>908</v>
       </c>
       <c r="L147" s="19"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>1022</v>
+        <v>912</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>1023</v>
+        <v>913</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>45</v>
+        <v>930</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E148" s="4">
         <v>44330</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>1024</v>
+        <v>918</v>
       </c>
       <c r="G148" s="11" t="s">
-        <v>1025</v>
+        <v>919</v>
       </c>
       <c r="H148" s="9" t="s">
-        <v>1026</v>
+        <v>920</v>
       </c>
       <c r="I148" s="9"/>
       <c r="J148" s="15" t="s">
-        <v>1027</v>
+        <v>925</v>
       </c>
       <c r="K148" s="19" t="s">
-        <v>1028</v>
+        <v>928</v>
       </c>
       <c r="L148" s="19"/>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>1002</v>
+        <v>909</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>1003</v>
+        <v>910</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>336</v>
+        <v>911</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>109</v>
+        <v>11</v>
       </c>
       <c r="E149" s="4">
         <v>44330</v>
       </c>
       <c r="F149" s="9" t="s">
-        <v>1009</v>
+        <v>916</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>1010</v>
-      </c>
-      <c r="H149" s="9" t="s">
-        <v>1011</v>
-      </c>
+        <v>917</v>
+      </c>
+      <c r="H149" s="9"/>
       <c r="I149" s="9"/>
       <c r="J149" s="15" t="s">
-        <v>1014</v>
+        <v>943</v>
       </c>
       <c r="K149" s="19" t="s">
-        <v>1016</v>
-      </c>
-      <c r="L149" s="23" t="s">
-        <v>1017</v>
-      </c>
+        <v>927</v>
+      </c>
+      <c r="L149" s="19"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>953</v>
+        <v>1020</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>954</v>
+        <v>1021</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>627</v>
+        <v>45</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>408</v>
+        <v>29</v>
       </c>
       <c r="E150" s="4">
         <v>44330</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>967</v>
+        <v>1022</v>
       </c>
       <c r="G150" s="11" t="s">
-        <v>968</v>
-      </c>
-      <c r="H150" s="9"/>
+        <v>1023</v>
+      </c>
+      <c r="H150" s="9" t="s">
+        <v>1024</v>
+      </c>
       <c r="I150" s="9"/>
       <c r="J150" s="15" t="s">
-        <v>981</v>
+        <v>1025</v>
       </c>
       <c r="K150" s="19" t="s">
-        <v>986</v>
+        <v>1026</v>
       </c>
       <c r="L150" s="19"/>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>933</v>
+        <v>1001</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>934</v>
+        <v>1002</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>39</v>
+        <v>336</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>19</v>
+        <v>109</v>
       </c>
       <c r="E151" s="4">
-        <v>44333</v>
+        <v>44330</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>938</v>
+        <v>1008</v>
       </c>
       <c r="G151" s="11" t="s">
-        <v>939</v>
+        <v>1009</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>1001</v>
+        <v>1010</v>
       </c>
       <c r="I151" s="9"/>
       <c r="J151" s="15" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="K151" s="19" t="s">
-        <v>947</v>
-      </c>
-      <c r="L151" s="19" t="s">
-        <v>948</v>
+        <v>1093</v>
+      </c>
+      <c r="L151" s="23" t="s">
+        <v>1015</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>141</v>
+        <v>952</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>955</v>
-      </c>
-      <c r="C152" s="2"/>
+        <v>953</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>627</v>
+      </c>
       <c r="D152" s="2" t="s">
-        <v>143</v>
+        <v>408</v>
       </c>
       <c r="E152" s="4">
-        <v>44335</v>
+        <v>44330</v>
       </c>
       <c r="F152" s="9" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="G152" s="11" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="H152" s="9"/>
       <c r="I152" s="9"/>
-      <c r="J152" s="15"/>
-      <c r="K152" s="19"/>
+      <c r="J152" s="15" t="s">
+        <v>980</v>
+      </c>
+      <c r="K152" s="19" t="s">
+        <v>985</v>
+      </c>
       <c r="L152" s="19"/>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>958</v>
+        <v>932</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>959</v>
+        <v>933</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>335</v>
+        <v>39</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E153" s="4">
-        <v>44337</v>
-      </c>
-      <c r="F153" s="11" t="s">
-        <v>974</v>
-      </c>
-      <c r="G153" s="9" t="s">
-        <v>1021</v>
+        <v>44333</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>937</v>
+      </c>
+      <c r="G153" s="11" t="s">
+        <v>938</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>973</v>
-      </c>
-      <c r="I153" s="9" t="s">
-        <v>975</v>
-      </c>
+        <v>1000</v>
+      </c>
+      <c r="I153" s="9"/>
       <c r="J153" s="15" t="s">
-        <v>982</v>
+        <v>1017</v>
       </c>
       <c r="K153" s="19" t="s">
-        <v>988</v>
-      </c>
-      <c r="L153" s="19"/>
+        <v>946</v>
+      </c>
+      <c r="L153" s="19" t="s">
+        <v>947</v>
+      </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>996</v>
+        <v>141</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>997</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D154" s="22" t="s">
-        <v>998</v>
+        <v>954</v>
+      </c>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="E154" s="4">
-        <v>44337</v>
+        <v>44335</v>
       </c>
       <c r="F154" s="9" t="s">
-        <v>1004</v>
+        <v>968</v>
       </c>
       <c r="G154" s="11" t="s">
-        <v>1005</v>
-      </c>
-      <c r="H154" s="9" t="s">
-        <v>1006</v>
-      </c>
+        <v>969</v>
+      </c>
+      <c r="H154" s="9"/>
       <c r="I154" s="9"/>
-      <c r="J154" s="15" t="s">
-        <v>1012</v>
-      </c>
-      <c r="K154" s="19" t="s">
-        <v>1015</v>
-      </c>
+      <c r="J154" s="15"/>
+      <c r="K154" s="19"/>
       <c r="L154" s="19"/>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>711</v>
+        <v>957</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>713</v>
+        <v>335</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>957</v>
+        <v>8</v>
       </c>
       <c r="E155" s="4">
         <v>44337</v>
       </c>
-      <c r="F155" s="9" t="s">
-        <v>971</v>
-      </c>
-      <c r="G155" s="11" t="s">
+      <c r="F155" s="11" t="s">
+        <v>973</v>
+      </c>
+      <c r="G155" s="9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="H155" s="9" t="s">
         <v>972</v>
       </c>
-      <c r="H155" s="9"/>
-      <c r="I155" s="9"/>
+      <c r="I155" s="9" t="s">
+        <v>974</v>
+      </c>
       <c r="J155" s="15" t="s">
-        <v>1020</v>
+        <v>981</v>
       </c>
       <c r="K155" s="19" t="s">
         <v>987</v>
@@ -8748,80 +8875,286 @@
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>989</v>
+        <v>995</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="D156" s="22" t="s">
+        <v>997</v>
       </c>
       <c r="E156" s="4">
         <v>44337</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>991</v>
+        <v>1003</v>
       </c>
       <c r="G156" s="11" t="s">
-        <v>992</v>
+        <v>1004</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>993</v>
+        <v>1005</v>
       </c>
       <c r="I156" s="9"/>
-      <c r="J156" s="15"/>
+      <c r="J156" s="15" t="s">
+        <v>1011</v>
+      </c>
       <c r="K156" s="19" t="s">
-        <v>994</v>
+        <v>1014</v>
       </c>
       <c r="L156" s="19"/>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>1029</v>
+        <v>711</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>1030</v>
+        <v>955</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>1031</v>
+        <v>713</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>29</v>
+        <v>956</v>
       </c>
       <c r="E157" s="4">
-        <v>44344</v>
+        <v>44337</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>1039</v>
+        <v>970</v>
       </c>
       <c r="G157" s="11" t="s">
-        <v>1040</v>
+        <v>971</v>
       </c>
       <c r="H157" s="9"/>
       <c r="I157" s="9"/>
       <c r="J157" s="15" t="s">
+        <v>1018</v>
+      </c>
+      <c r="K157" s="19" t="s">
+        <v>986</v>
+      </c>
+      <c r="L157" s="19"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E158" s="4">
+        <v>44337</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G158" s="11" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H158" s="9" t="s">
+        <v>1077</v>
+      </c>
+      <c r="I158" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="J158" s="15" t="s">
+        <v>1084</v>
+      </c>
+      <c r="K158" s="19" t="s">
+        <v>1091</v>
+      </c>
+      <c r="L158" s="19"/>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D159" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E159" s="4">
+        <v>44337</v>
+      </c>
+      <c r="F159" s="9" t="s">
+        <v>990</v>
+      </c>
+      <c r="G159" s="11" t="s">
+        <v>991</v>
+      </c>
+      <c r="H159" s="9" t="s">
+        <v>992</v>
+      </c>
+      <c r="I159" s="9"/>
+      <c r="J159" s="15"/>
+      <c r="K159" s="19" t="s">
+        <v>993</v>
+      </c>
+      <c r="L159" s="19"/>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E160" s="4">
+        <v>44344</v>
+      </c>
+      <c r="F160" s="9" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G160" s="11" t="s">
+        <v>1038</v>
+      </c>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="15" t="s">
+        <v>1044</v>
+      </c>
+      <c r="K160" s="19" t="s">
         <v>1046</v>
       </c>
-      <c r="K157" s="19" t="s">
-        <v>1048</v>
-      </c>
-      <c r="L157" s="19"/>
+      <c r="L160" s="19"/>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E161" s="4">
+        <v>44351</v>
+      </c>
+      <c r="F161" s="9" t="s">
+        <v>1069</v>
+      </c>
+      <c r="G161" s="11" t="s">
+        <v>1070</v>
+      </c>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="15"/>
+      <c r="K161" s="19" t="s">
+        <v>1089</v>
+      </c>
+      <c r="L161" s="19"/>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E162" s="4">
+        <v>44351</v>
+      </c>
+      <c r="F162" s="9" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G162" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="H162" s="11" t="s">
+        <v>1073</v>
+      </c>
+      <c r="I162" s="9" t="s">
+        <v>1071</v>
+      </c>
+      <c r="J162" s="15" t="s">
+        <v>1083</v>
+      </c>
+      <c r="K162" s="19" t="s">
+        <v>1090</v>
+      </c>
+      <c r="L162" s="19"/>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D163" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E163" s="4">
+        <v>44357</v>
+      </c>
+      <c r="F163" s="9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="G163" s="11" t="s">
+        <v>1066</v>
+      </c>
+      <c r="H163" s="9" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I163" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="J163" s="15" t="s">
+        <v>1082</v>
+      </c>
+      <c r="K163" s="19" t="s">
+        <v>1087</v>
+      </c>
+      <c r="L163" s="19" t="s">
+        <v>1088</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L157" xr:uid="{16139DE7-2F8E-49DC-B7F8-DD7F1B9622C0}">
+  <autoFilter ref="A1:L163" xr:uid="{16139DE7-2F8E-49DC-B7F8-DD7F1B9622C0}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L150">
       <sortCondition ref="E2:E150"/>
       <sortCondition ref="B2:B150"/>
       <sortCondition ref="A2:A150"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L157">
-    <sortCondition ref="E2:E157"/>
-    <sortCondition ref="B2:B157"/>
-    <sortCondition ref="A2:A157"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L163">
+    <sortCondition ref="E2:E163"/>
+    <sortCondition ref="B2:B163"/>
+    <sortCondition ref="A2:A163"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>